<commit_message>
Update that input of CQ works
</commit_message>
<xml_diff>
--- a/CQ_Plate/CQ_InputTemplate.xlsx
+++ b/CQ_Plate/CQ_InputTemplate.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\MSc Leiden 2nd Year\##LabAst Works\ot2\CQ_Plate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jornb\Documents\GitHub\ot2\CQ_Plate\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2F437F-EFC9-49F6-B39A-892472090739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="32700" yWindow="2475" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +26,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="59">
   <si>
     <t>Drug Name</t>
   </si>
@@ -153,12 +157,6 @@
     <t>AB3</t>
   </si>
   <si>
-    <t>Medium-A</t>
-  </si>
-  <si>
-    <t>Medium-B</t>
-  </si>
-  <si>
     <t>AB1_AB2_AB3</t>
   </si>
   <si>
@@ -235,12 +233,15 @@
   </si>
   <si>
     <t>16_0_1</t>
+  </si>
+  <si>
+    <t>MED-A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,7 +367,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -677,11 +678,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,34 +882,34 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M11" s="2"/>
       <c r="O11" s="11" t="s">
@@ -921,34 +922,34 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M12" s="2"/>
     </row>
@@ -958,34 +959,34 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M13" s="2"/>
     </row>
@@ -995,34 +996,34 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M14" s="2"/>
     </row>
@@ -1032,34 +1033,34 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M15" s="2"/>
     </row>
@@ -1069,34 +1070,34 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M16" s="2"/>
     </row>
@@ -1212,34 +1213,34 @@
         <v>0</v>
       </c>
       <c r="C22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="H22" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L22" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="M22" s="14">
         <v>0</v>
@@ -1256,34 +1257,34 @@
         <v>0</v>
       </c>
       <c r="C23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="I23" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="J23" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="K23" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G23" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="K23" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="L23" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M23" s="14">
         <v>0</v>
@@ -1297,34 +1298,34 @@
         <v>0</v>
       </c>
       <c r="C24" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="I24" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="J24" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="K24" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="L24" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M24" s="14">
         <v>0</v>
@@ -1338,34 +1339,34 @@
         <v>0</v>
       </c>
       <c r="C25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="I25" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="J25" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="K25" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G25" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="K25" s="14" t="s">
-        <v>51</v>
-      </c>
       <c r="L25" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M25" s="14">
         <v>0</v>
@@ -1379,34 +1380,34 @@
         <v>0</v>
       </c>
       <c r="C26" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="I26" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="J26" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="K26" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="L26" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M26" s="14">
         <v>0</v>
@@ -1420,34 +1421,34 @@
         <v>0</v>
       </c>
       <c r="C27" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="I27" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="J27" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="K27" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G27" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J27" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="L27" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M27" s="14">
         <v>0</v>
@@ -1542,40 +1543,40 @@
         <v>5</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="O33" s="11" t="s">
         <v>22</v>
@@ -1586,40 +1587,40 @@
         <v>6</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -1627,40 +1628,40 @@
         <v>7</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -1668,40 +1669,40 @@
         <v>8</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -1709,40 +1710,40 @@
         <v>9</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -1750,40 +1751,40 @@
         <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -1791,40 +1792,40 @@
         <v>11</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -1832,40 +1833,40 @@
         <v>12</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -2213,51 +2214,51 @@
       </c>
       <c r="B57" s="4" t="str">
         <f>CONCATENATE(B10," ",B21," ",B33," ",B45)</f>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="C57" s="4" t="str">
         <f t="shared" ref="C57:M57" si="0">CONCATENATE(C10," ",C21," ",C33," ",C45)</f>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="D57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="E57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="F57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="G57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="H57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="I57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="J57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="K57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="L57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="M57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2266,51 +2267,51 @@
       </c>
       <c r="B58" s="4" t="str">
         <f t="shared" ref="B58:M64" si="1">CONCATENATE(B11," ",B22," ",B34," ",B46)</f>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="C58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_32_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_32_0 MED-A STR</v>
       </c>
       <c r="D58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_32_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_32_0 MED-A STR</v>
       </c>
       <c r="E58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_32_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_32_0 MED-A STR</v>
       </c>
       <c r="F58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_32_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_32_0 MED-A STR</v>
       </c>
       <c r="G58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 0_0_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 0_0_0 MED-A STR</v>
       </c>
       <c r="H58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_32 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_32 MED-A STR</v>
       </c>
       <c r="I58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_32 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_32 MED-A STR</v>
       </c>
       <c r="J58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_32 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_32 MED-A STR</v>
       </c>
       <c r="K58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_32 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_32 MED-A STR</v>
       </c>
       <c r="L58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 0_0_0 Medium-B STR</v>
+        <v>AB1_AB2_AB3 0_0_0 MED-A STR</v>
       </c>
       <c r="M58" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2319,51 +2320,51 @@
       </c>
       <c r="B59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="C59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_16_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_16_0 MED-A STR</v>
       </c>
       <c r="D59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_16_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_16_0 MED-A STR</v>
       </c>
       <c r="E59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_16_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_16_0 MED-A STR</v>
       </c>
       <c r="F59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_16_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_16_0 MED-A STR</v>
       </c>
       <c r="G59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 0_0_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 0_0_0 MED-A STR</v>
       </c>
       <c r="H59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_16 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_16 MED-A STR</v>
       </c>
       <c r="I59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_16 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_16 MED-A STR</v>
       </c>
       <c r="J59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_16 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_16 MED-A STR</v>
       </c>
       <c r="K59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_16 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_16 MED-A STR</v>
       </c>
       <c r="L59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 0_0_0 Medium-B STR</v>
+        <v>AB1_AB2_AB3 0_0_0 MED-A STR</v>
       </c>
       <c r="M59" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2372,51 +2373,51 @@
       </c>
       <c r="B60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="C60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_8_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_8_0 MED-A STR</v>
       </c>
       <c r="D60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_8_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_8_0 MED-A STR</v>
       </c>
       <c r="E60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_8_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_8_0 MED-A STR</v>
       </c>
       <c r="F60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_8_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_8_0 MED-A STR</v>
       </c>
       <c r="G60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 0_0_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 0_0_0 MED-A STR</v>
       </c>
       <c r="H60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_8 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_8 MED-A STR</v>
       </c>
       <c r="I60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_8 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_8 MED-A STR</v>
       </c>
       <c r="J60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_8 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_8 MED-A STR</v>
       </c>
       <c r="K60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_8 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_8 MED-A STR</v>
       </c>
       <c r="L60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 0_0_0 Medium-B STR</v>
+        <v>AB1_AB2_AB3 0_0_0 MED-A STR</v>
       </c>
       <c r="M60" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,51 +2426,51 @@
       </c>
       <c r="B61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="C61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_4_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_4_0 MED-A STR</v>
       </c>
       <c r="D61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_4_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_4_0 MED-A STR</v>
       </c>
       <c r="E61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_4_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_4_0 MED-A STR</v>
       </c>
       <c r="F61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_4_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_4_0 MED-A STR</v>
       </c>
       <c r="G61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 Medium-A </v>
+        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 MED-A </v>
       </c>
       <c r="H61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_4 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_4 MED-A STR</v>
       </c>
       <c r="I61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_4 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_4 MED-A STR</v>
       </c>
       <c r="J61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_4 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_4 MED-A STR</v>
       </c>
       <c r="K61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_4 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_4 MED-A STR</v>
       </c>
       <c r="L61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 Medium-B </v>
+        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 MED-A </v>
       </c>
       <c r="M61" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2478,51 +2479,51 @@
       </c>
       <c r="B62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="C62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_2_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_2_0 MED-A STR</v>
       </c>
       <c r="D62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_2_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_2_0 MED-A STR</v>
       </c>
       <c r="E62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_2_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_2_0 MED-A STR</v>
       </c>
       <c r="F62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_2_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_2_0 MED-A STR</v>
       </c>
       <c r="G62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 Medium-A </v>
+        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 MED-A </v>
       </c>
       <c r="H62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_2 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_2 MED-A STR</v>
       </c>
       <c r="I62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_2 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_2 MED-A STR</v>
       </c>
       <c r="J62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_2 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_2 MED-A STR</v>
       </c>
       <c r="K62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_2 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_2 MED-A STR</v>
       </c>
       <c r="L62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 Medium-B </v>
+        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 MED-A </v>
       </c>
       <c r="M62" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2531,51 +2532,51 @@
       </c>
       <c r="B63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="C63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_1_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_1_0 MED-A STR</v>
       </c>
       <c r="D63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_1_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 32_1_0 MED-A STR</v>
       </c>
       <c r="E63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_1_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_1_0 MED-A STR</v>
       </c>
       <c r="F63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_1_0 Medium-A STR</v>
+        <v>AB1_AB2_AB3 16_1_0 MED-A STR</v>
       </c>
       <c r="G63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 Medium-A </v>
+        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 MED-A </v>
       </c>
       <c r="H63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_1 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_1 MED-A STR</v>
       </c>
       <c r="I63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 32_0_1 Medium-B STR</v>
+        <v>AB1_AB2_AB3 32_0_1 MED-A STR</v>
       </c>
       <c r="J63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_1 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_1 MED-A STR</v>
       </c>
       <c r="K63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>AB1_AB2_AB3 16_0_1 Medium-B STR</v>
+        <v>AB1_AB2_AB3 16_0_1 MED-A STR</v>
       </c>
       <c r="L63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 Medium-B </v>
+        <v xml:space="preserve">AB1_AB2_AB3 0_0_0 MED-A </v>
       </c>
       <c r="M63" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2584,56 +2585,56 @@
       </c>
       <c r="B64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="C64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="D64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="E64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="F64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="G64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-A </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="H64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="I64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="J64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="K64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="L64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
       <c r="M64" s="4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> 0 Medium-B </v>
+        <v xml:space="preserve"> 0 MED-A </v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$O$2:$O$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>